<commit_message>
in progress luce plan
</commit_message>
<xml_diff>
--- a/xls/luceplan/luceplan_originario.xlsx
+++ b/xls/luceplan/luceplan_originario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38140" yWindow="-4540" windowWidth="35200" windowHeight="17320"/>
+    <workbookView xWindow="4660" yWindow="1920" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="541">
   <si>
     <t>Descrizione</t>
   </si>
@@ -1645,6 +1645,15 @@
   </si>
   <si>
     <t xml:space="preserve">Dimensioni </t>
+  </si>
+  <si>
+    <t>1D30/0600025,1D30/0200004,1D30/04/0125,1D30/04/0225,1D30/04/0325,1D30/0500004</t>
+  </si>
+  <si>
+    <t>1D170Q/01023,1D170Q/01024,1D170Q/01027,1D170Q/01036,1D170Q/02020</t>
+  </si>
+  <si>
+    <t>Accessori</t>
   </si>
 </sst>
 </file>
@@ -1734,7 +1743,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1751,6 +1760,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2058,7 +2073,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2068,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J120" sqref="J120"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2081,9 +2096,11 @@
     <col min="7" max="7" width="31.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.83203125" customWidth="1"/>
+    <col min="13" max="13" width="14.83203125" customWidth="1"/>
+    <col min="14" max="14" width="31.1640625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15">
+    <row r="1" spans="1:14" ht="15">
       <c r="A1" s="1" t="s">
         <v>529</v>
       </c>
@@ -2123,8 +2140,11 @@
       <c r="M1" s="3" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2150,8 +2170,9 @@
       <c r="M2" s="7">
         <v>62.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2" s="15"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -2179,8 +2200,11 @@
       <c r="M3" s="7">
         <v>282.79000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -2208,8 +2232,11 @@
       <c r="M4" s="7">
         <v>336.89</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -2237,8 +2264,11 @@
       <c r="M5" s="7">
         <v>361.48</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="4" t="s">
         <v>28</v>
       </c>
@@ -2264,8 +2294,9 @@
       <c r="M6" s="7">
         <v>510.66</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6" s="15"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -2294,8 +2325,9 @@
       <c r="M7" s="7">
         <v>347.54</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7" s="15"/>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
@@ -2324,8 +2356,9 @@
       <c r="M8" s="7">
         <v>293.44</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
@@ -2354,8 +2387,9 @@
       <c r="M9" s="7">
         <v>431.15</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
         <v>50</v>
       </c>
@@ -2384,8 +2418,9 @@
       <c r="M10" s="7">
         <v>379.51</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="4" t="s">
         <v>56</v>
       </c>
@@ -2416,8 +2451,9 @@
       <c r="M11" s="7">
         <v>347.54</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11" s="15"/>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="4" t="s">
         <v>64</v>
       </c>
@@ -2448,8 +2484,9 @@
       <c r="M12" s="7">
         <v>347.54</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12" s="15"/>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="4" t="s">
         <v>67</v>
       </c>
@@ -2480,8 +2517,9 @@
       <c r="M13" s="7">
         <v>335.25</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13" s="15"/>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="4" t="s">
         <v>71</v>
       </c>
@@ -2512,8 +2550,9 @@
       <c r="M14" s="7">
         <v>335.25</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" s="15"/>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="4" t="s">
         <v>73</v>
       </c>
@@ -2541,8 +2580,9 @@
       <c r="M15" s="7">
         <v>1340.16</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="4" t="s">
         <v>79</v>
       </c>
@@ -2570,8 +2610,9 @@
       <c r="M16" s="7">
         <v>1340.16</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" s="15"/>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="4" t="s">
         <v>82</v>
       </c>
@@ -2597,8 +2638,9 @@
       <c r="M17" s="7">
         <v>333.61</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="4" t="s">
         <v>87</v>
       </c>
@@ -2626,8 +2668,9 @@
       <c r="M18" s="7">
         <v>875.41</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" s="16"/>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="4" t="s">
         <v>94</v>
       </c>
@@ -2655,8 +2698,9 @@
       <c r="M19" s="7">
         <v>875.41</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" s="16"/>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="4" t="s">
         <v>96</v>
       </c>
@@ -2684,8 +2728,9 @@
       <c r="M20" s="7">
         <v>875.41</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20" s="16"/>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="4" t="s">
         <v>99</v>
       </c>
@@ -2713,8 +2758,9 @@
       <c r="M21" s="7">
         <v>899.18</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" s="15"/>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="4" t="s">
         <v>105</v>
       </c>
@@ -2742,8 +2788,9 @@
       <c r="M22" s="7">
         <v>899.18</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22" s="15"/>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="4" t="s">
         <v>107</v>
       </c>
@@ -2771,8 +2818,9 @@
       <c r="M23" s="7">
         <v>899.18</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="4" t="s">
         <v>109</v>
       </c>
@@ -2798,8 +2846,9 @@
       <c r="M24" s="7">
         <v>177.05</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="N24" s="15"/>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="4" t="s">
         <v>116</v>
       </c>
@@ -2827,8 +2876,9 @@
       <c r="M25" s="7">
         <v>724.59</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25" s="15"/>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="4" t="s">
         <v>120</v>
       </c>
@@ -2856,8 +2906,9 @@
       <c r="M26" s="7">
         <v>724.59</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26" s="15"/>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="4" t="s">
         <v>123</v>
       </c>
@@ -2885,8 +2936,9 @@
       <c r="M27" s="7">
         <v>365.57</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27" s="15"/>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="4" t="s">
         <v>129</v>
       </c>
@@ -2914,8 +2966,9 @@
       <c r="M28" s="7">
         <v>365.57</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28" s="15"/>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="4" t="s">
         <v>131</v>
       </c>
@@ -2941,8 +2994,11 @@
       <c r="M29" s="7">
         <v>407.38</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="N29" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="4" t="s">
         <v>135</v>
       </c>
@@ -2970,8 +3026,9 @@
       <c r="M30" s="7">
         <v>262.3</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="N30" s="15"/>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="4" t="s">
         <v>142</v>
       </c>
@@ -2999,8 +3056,9 @@
       <c r="M31" s="7">
         <v>262.3</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="N31" s="15"/>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="4" t="s">
         <v>145</v>
       </c>
@@ -3029,8 +3087,9 @@
       <c r="M32" s="7">
         <v>860.66</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32" s="15"/>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="4" t="s">
         <v>152</v>
       </c>
@@ -3059,8 +3118,9 @@
       <c r="M33" s="7">
         <v>890.98</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="N33" s="15"/>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="4" t="s">
         <v>157</v>
       </c>
@@ -3088,8 +3148,9 @@
       <c r="M34" s="7">
         <v>176.23</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="N34" s="15"/>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="4" t="s">
         <v>164</v>
       </c>
@@ -3117,8 +3178,9 @@
       <c r="M35" s="7">
         <v>176.23</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="N35" s="15"/>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="4" t="s">
         <v>167</v>
       </c>
@@ -3146,8 +3208,9 @@
       <c r="M36" s="7">
         <v>240.98</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="N36" s="15"/>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="4" t="s">
         <v>173</v>
       </c>
@@ -3175,8 +3238,9 @@
       <c r="M37" s="7">
         <v>321.31</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="N37" s="15"/>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" s="4" t="s">
         <v>176</v>
       </c>
@@ -3204,8 +3268,9 @@
       <c r="M38" s="7">
         <v>282.79000000000002</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="N38" s="15"/>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="4" t="s">
         <v>184</v>
       </c>
@@ -3233,8 +3298,9 @@
       <c r="M39" s="7">
         <v>658.2</v>
       </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="N39" s="15"/>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" s="4" t="s">
         <v>190</v>
       </c>
@@ -3262,8 +3328,9 @@
       <c r="M40" s="7">
         <v>9489.34</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="N40" s="15"/>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" s="4" t="s">
         <v>196</v>
       </c>
@@ -3291,8 +3358,9 @@
       <c r="M41" s="7">
         <v>957.38</v>
       </c>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="N41" s="15"/>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" s="4" t="s">
         <v>203</v>
       </c>
@@ -3320,8 +3388,9 @@
       <c r="M42" s="7">
         <v>853.28</v>
       </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="N42" s="15"/>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" s="4" t="s">
         <v>207</v>
       </c>
@@ -3349,8 +3418,9 @@
       <c r="M43" s="7">
         <v>1133.6099999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="N43" s="15"/>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" s="4" t="s">
         <v>212</v>
       </c>
@@ -3375,8 +3445,9 @@
       <c r="M44" s="7">
         <v>1203.28</v>
       </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="N44" s="15"/>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" s="4" t="s">
         <v>217</v>
       </c>
@@ -3401,8 +3472,9 @@
       <c r="M45" s="7">
         <v>490.16</v>
       </c>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="N45" s="15"/>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" s="4" t="s">
         <v>222</v>
       </c>
@@ -3427,8 +3499,9 @@
       <c r="M46" s="7">
         <v>1154.92</v>
       </c>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="N46" s="15"/>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" s="4" t="s">
         <v>227</v>
       </c>
@@ -3456,8 +3529,9 @@
       <c r="M47" s="7">
         <v>2367.21</v>
       </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="N47" s="15"/>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" s="4" t="s">
         <v>232</v>
       </c>
@@ -3485,8 +3559,9 @@
       <c r="M48" s="7">
         <v>3417.21</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="N48" s="15"/>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" s="4" t="s">
         <v>237</v>
       </c>
@@ -3512,8 +3587,9 @@
       <c r="M49" s="7">
         <v>272.13</v>
       </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="N49" s="15"/>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" s="4" t="s">
         <v>242</v>
       </c>
@@ -3539,8 +3615,9 @@
       <c r="M50" s="7">
         <v>189.34</v>
       </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="N50" s="15"/>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" s="10" t="s">
         <v>248</v>
       </c>
@@ -3574,8 +3651,11 @@
       <c r="M51" s="12">
         <v>2650.82</v>
       </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="N51" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" s="10" t="s">
         <v>256</v>
       </c>
@@ -3609,8 +3689,11 @@
       <c r="M52" s="12">
         <v>2748.36</v>
       </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="N52" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" s="10" t="s">
         <v>261</v>
       </c>
@@ -3644,8 +3727,11 @@
       <c r="M53" s="12">
         <v>2748.36</v>
       </c>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="N53" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" s="10" t="s">
         <v>266</v>
       </c>
@@ -3679,8 +3765,11 @@
       <c r="M54" s="12">
         <v>2748.36</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="N54" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" s="10" t="s">
         <v>271</v>
       </c>
@@ -3714,8 +3803,11 @@
       <c r="M55" s="12">
         <v>2748.36</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="N55" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56" s="10" t="s">
         <v>276</v>
       </c>
@@ -3749,8 +3841,11 @@
       <c r="M56" s="12">
         <v>3413.11</v>
       </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="N56" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" s="10" t="s">
         <v>281</v>
       </c>
@@ -3784,8 +3879,11 @@
       <c r="M57" s="12">
         <v>3498.36</v>
       </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="N57" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" s="10" t="s">
         <v>285</v>
       </c>
@@ -3819,8 +3917,11 @@
       <c r="M58" s="12">
         <v>3498.36</v>
       </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="N58" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" s="10" t="s">
         <v>289</v>
       </c>
@@ -3854,8 +3955,11 @@
       <c r="M59" s="12">
         <v>3498.36</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="N59" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" s="10" t="s">
         <v>293</v>
       </c>
@@ -3889,8 +3993,11 @@
       <c r="M60" s="12">
         <v>3498.36</v>
       </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="N60" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" s="10" t="s">
         <v>297</v>
       </c>
@@ -3924,8 +4031,11 @@
       <c r="M61" s="12">
         <v>2726.23</v>
       </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="N61" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" s="10" t="s">
         <v>302</v>
       </c>
@@ -3959,8 +4069,11 @@
       <c r="M62" s="12">
         <v>2868.85</v>
       </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="N62" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" s="10" t="s">
         <v>306</v>
       </c>
@@ -3994,8 +4107,11 @@
       <c r="M63" s="12">
         <v>2868.85</v>
       </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="N63" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" s="10" t="s">
         <v>310</v>
       </c>
@@ -4029,8 +4145,11 @@
       <c r="M64" s="12">
         <v>2868.85</v>
       </c>
-    </row>
-    <row r="65" spans="1:13">
+      <c r="N64" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" s="10" t="s">
         <v>314</v>
       </c>
@@ -4064,8 +4183,11 @@
       <c r="M65" s="12">
         <v>2868.85</v>
       </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="N65" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
       <c r="A66" s="10" t="s">
         <v>318</v>
       </c>
@@ -4099,8 +4221,11 @@
       <c r="M66" s="12">
         <v>3425.41</v>
       </c>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="N66" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
       <c r="A67" s="10" t="s">
         <v>322</v>
       </c>
@@ -4134,8 +4259,11 @@
       <c r="M67" s="12">
         <v>3568.03</v>
       </c>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="N67" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
       <c r="A68" s="10" t="s">
         <v>326</v>
       </c>
@@ -4169,8 +4297,11 @@
       <c r="M68" s="12">
         <v>3568.03</v>
       </c>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="N68" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
       <c r="A69" s="10" t="s">
         <v>330</v>
       </c>
@@ -4204,8 +4335,11 @@
       <c r="M69" s="12">
         <v>3568.03</v>
       </c>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="N69" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
       <c r="A70" s="10" t="s">
         <v>334</v>
       </c>
@@ -4239,8 +4373,11 @@
       <c r="M70" s="12">
         <v>3568.03</v>
       </c>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="N70" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
       <c r="A71" s="10" t="s">
         <v>338</v>
       </c>
@@ -4268,8 +4405,9 @@
       <c r="M71" s="12">
         <v>104.1</v>
       </c>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="N71" s="15"/>
+    </row>
+    <row r="72" spans="1:14">
       <c r="A72" s="4" t="s">
         <v>344</v>
       </c>
@@ -4295,8 +4433,14 @@
       <c r="K72" s="9" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="M72" s="14">
+        <v>1477.05</v>
+      </c>
+      <c r="N72" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14">
       <c r="A73" s="4" t="s">
         <v>348</v>
       </c>
@@ -4322,8 +4466,14 @@
       <c r="K73" s="9" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="M73" s="14">
+        <v>1590.98</v>
+      </c>
+      <c r="N73" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
       <c r="A74" s="4" t="s">
         <v>351</v>
       </c>
@@ -4343,8 +4493,12 @@
       <c r="G74" s="4" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="M74" s="14">
+        <v>2235.25</v>
+      </c>
+      <c r="N74" s="15"/>
+    </row>
+    <row r="75" spans="1:14">
       <c r="A75" s="4" t="s">
         <v>355</v>
       </c>
@@ -4372,8 +4526,9 @@
       <c r="M75" s="7">
         <v>840.16</v>
       </c>
-    </row>
-    <row r="76" spans="1:13">
+      <c r="N75" s="15"/>
+    </row>
+    <row r="76" spans="1:14">
       <c r="A76" s="4" t="s">
         <v>360</v>
       </c>
@@ -4399,8 +4554,9 @@
       <c r="M76" s="7">
         <v>31.15</v>
       </c>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="N76" s="15"/>
+    </row>
+    <row r="77" spans="1:14">
       <c r="A77" s="4" t="s">
         <v>367</v>
       </c>
@@ -4429,8 +4585,9 @@
       <c r="M77" s="7">
         <v>22.95</v>
       </c>
-    </row>
-    <row r="78" spans="1:13">
+      <c r="N77" s="15"/>
+    </row>
+    <row r="78" spans="1:14">
       <c r="A78" s="4" t="s">
         <v>373</v>
       </c>
@@ -4459,8 +4616,9 @@
       <c r="M78" s="7">
         <v>43.44</v>
       </c>
-    </row>
-    <row r="79" spans="1:13">
+      <c r="N78" s="15"/>
+    </row>
+    <row r="79" spans="1:14">
       <c r="A79" s="4" t="s">
         <v>378</v>
       </c>
@@ -4489,8 +4647,9 @@
       <c r="M79" s="7">
         <v>56.56</v>
       </c>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="N79" s="15"/>
+    </row>
+    <row r="80" spans="1:14">
       <c r="A80" s="4" t="s">
         <v>383</v>
       </c>
@@ -4516,8 +4675,9 @@
       <c r="M80" s="7">
         <v>44.26</v>
       </c>
-    </row>
-    <row r="81" spans="1:13">
+      <c r="N80" s="15"/>
+    </row>
+    <row r="81" spans="1:14">
       <c r="A81" s="4" t="s">
         <v>388</v>
       </c>
@@ -4543,8 +4703,9 @@
       <c r="M81" s="7">
         <v>63.93</v>
       </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="N81" s="15"/>
+    </row>
+    <row r="82" spans="1:14">
       <c r="A82" s="4" t="s">
         <v>393</v>
       </c>
@@ -4572,8 +4733,11 @@
       <c r="M82" s="7">
         <v>126.23</v>
       </c>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="N82" s="15" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14">
       <c r="A83" s="4" t="s">
         <v>400</v>
       </c>
@@ -4601,8 +4765,11 @@
       <c r="M83" s="7">
         <v>126.23</v>
       </c>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="N83" s="15" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14">
       <c r="A84" s="4" t="s">
         <v>404</v>
       </c>
@@ -4630,8 +4797,11 @@
       <c r="M84" s="7">
         <v>126.23</v>
       </c>
-    </row>
-    <row r="85" spans="1:13">
+      <c r="N84" s="15" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14">
       <c r="A85" s="4" t="s">
         <v>408</v>
       </c>
@@ -4659,8 +4829,9 @@
       <c r="M85" s="7">
         <v>1674.59</v>
       </c>
-    </row>
-    <row r="86" spans="1:13">
+      <c r="N85" s="15"/>
+    </row>
+    <row r="86" spans="1:14">
       <c r="A86" s="4" t="s">
         <v>414</v>
       </c>
@@ -4688,8 +4859,9 @@
       <c r="M86" s="7">
         <v>1709.84</v>
       </c>
-    </row>
-    <row r="87" spans="1:13">
+      <c r="N86" s="15"/>
+    </row>
+    <row r="87" spans="1:14">
       <c r="A87" s="4" t="s">
         <v>417</v>
       </c>
@@ -4717,8 +4889,9 @@
       <c r="M87" s="7">
         <v>1674.59</v>
       </c>
-    </row>
-    <row r="88" spans="1:13">
+      <c r="N87" s="15"/>
+    </row>
+    <row r="88" spans="1:14">
       <c r="A88" s="4" t="s">
         <v>422</v>
       </c>
@@ -4746,8 +4919,9 @@
       <c r="M88" s="7">
         <v>1709.84</v>
       </c>
-    </row>
-    <row r="89" spans="1:13">
+      <c r="N88" s="15"/>
+    </row>
+    <row r="89" spans="1:14">
       <c r="A89" s="4" t="s">
         <v>424</v>
       </c>
@@ -4776,8 +4950,9 @@
       <c r="M89" s="7">
         <v>336.89</v>
       </c>
-    </row>
-    <row r="90" spans="1:13">
+      <c r="N89" s="15"/>
+    </row>
+    <row r="90" spans="1:14">
       <c r="A90" s="4" t="s">
         <v>432</v>
       </c>
@@ -4806,8 +4981,9 @@
       <c r="M90" s="7">
         <v>279.51</v>
       </c>
-    </row>
-    <row r="91" spans="1:13">
+      <c r="N90" s="15"/>
+    </row>
+    <row r="91" spans="1:14">
       <c r="A91" s="4" t="s">
         <v>437</v>
       </c>
@@ -4833,8 +5009,9 @@
       <c r="M91" s="7">
         <v>459.02</v>
       </c>
-    </row>
-    <row r="92" spans="1:13">
+      <c r="N91" s="15"/>
+    </row>
+    <row r="92" spans="1:14">
       <c r="A92" s="4" t="s">
         <v>442</v>
       </c>
@@ -4860,8 +5037,9 @@
       <c r="M92" s="7">
         <v>335.25</v>
       </c>
-    </row>
-    <row r="93" spans="1:13">
+      <c r="N92" s="15"/>
+    </row>
+    <row r="93" spans="1:14">
       <c r="A93" s="4" t="s">
         <v>447</v>
       </c>
@@ -4889,8 +5067,9 @@
       <c r="M93" s="7">
         <v>43.44</v>
       </c>
-    </row>
-    <row r="94" spans="1:13">
+      <c r="N93" s="15"/>
+    </row>
+    <row r="94" spans="1:14">
       <c r="A94" s="4" t="s">
         <v>455</v>
       </c>
@@ -4918,8 +5097,9 @@
       <c r="M94" s="7">
         <v>43.44</v>
       </c>
-    </row>
-    <row r="95" spans="1:13">
+      <c r="N94" s="15"/>
+    </row>
+    <row r="95" spans="1:14">
       <c r="A95" s="4" t="s">
         <v>458</v>
       </c>
@@ -4947,8 +5127,9 @@
       <c r="M95" s="7">
         <v>43.44</v>
       </c>
-    </row>
-    <row r="96" spans="1:13">
+      <c r="N95" s="15"/>
+    </row>
+    <row r="96" spans="1:14">
       <c r="A96" s="4" t="s">
         <v>461</v>
       </c>
@@ -4976,8 +5157,9 @@
       <c r="M96" s="7">
         <v>43.44</v>
       </c>
-    </row>
-    <row r="97" spans="1:13">
+      <c r="N96" s="15"/>
+    </row>
+    <row r="97" spans="1:14">
       <c r="A97" s="4" t="s">
         <v>464</v>
       </c>
@@ -5003,8 +5185,9 @@
       <c r="M97" s="7">
         <v>178.69</v>
       </c>
-    </row>
-    <row r="98" spans="1:13">
+      <c r="N97" s="15"/>
+    </row>
+    <row r="98" spans="1:14">
       <c r="A98" s="4" t="s">
         <v>469</v>
       </c>
@@ -5030,8 +5213,11 @@
       <c r="M98" s="7">
         <v>875.41</v>
       </c>
-    </row>
-    <row r="99" spans="1:13">
+      <c r="N98" s="15" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14">
       <c r="A99" s="4" t="s">
         <v>473</v>
       </c>
@@ -5057,8 +5243,9 @@
       <c r="M99" s="7">
         <v>367.21</v>
       </c>
-    </row>
-    <row r="100" spans="1:13">
+      <c r="N99" s="15"/>
+    </row>
+    <row r="100" spans="1:14">
       <c r="A100" s="4" t="s">
         <v>479</v>
       </c>
@@ -5084,8 +5271,9 @@
       <c r="M100" s="7">
         <v>377.05</v>
       </c>
-    </row>
-    <row r="101" spans="1:13">
+      <c r="N100" s="15"/>
+    </row>
+    <row r="101" spans="1:14">
       <c r="A101" s="4" t="s">
         <v>485</v>
       </c>
@@ -5111,8 +5299,9 @@
       <c r="M101" s="7">
         <v>416.39</v>
       </c>
-    </row>
-    <row r="102" spans="1:13">
+      <c r="N101" s="15"/>
+    </row>
+    <row r="102" spans="1:14">
       <c r="A102" s="4" t="s">
         <v>491</v>
       </c>
@@ -5138,8 +5327,9 @@
       <c r="M102" s="7">
         <v>421.31</v>
       </c>
-    </row>
-    <row r="103" spans="1:13">
+      <c r="N102" s="15"/>
+    </row>
+    <row r="103" spans="1:14">
       <c r="A103" s="4" t="s">
         <v>496</v>
       </c>
@@ -5168,8 +5358,9 @@
       <c r="M103" s="7">
         <v>560.66</v>
       </c>
-    </row>
-    <row r="104" spans="1:13">
+      <c r="N103" s="15"/>
+    </row>
+    <row r="104" spans="1:14">
       <c r="A104" s="4" t="s">
         <v>502</v>
       </c>
@@ -5198,8 +5389,9 @@
       <c r="M104" s="7">
         <v>527.04999999999995</v>
       </c>
-    </row>
-    <row r="105" spans="1:13">
+      <c r="N104" s="15"/>
+    </row>
+    <row r="105" spans="1:14">
       <c r="A105" s="4" t="s">
         <v>506</v>
       </c>
@@ -5228,8 +5420,9 @@
       <c r="M105" s="7">
         <v>1026.23</v>
       </c>
-    </row>
-    <row r="106" spans="1:13">
+      <c r="N105" s="15"/>
+    </row>
+    <row r="106" spans="1:14">
       <c r="A106" s="4" t="s">
         <v>511</v>
       </c>
@@ -5258,8 +5451,9 @@
       <c r="M106" s="7">
         <v>1017.21</v>
       </c>
-    </row>
-    <row r="107" spans="1:13">
+      <c r="N106" s="15"/>
+    </row>
+    <row r="107" spans="1:14">
       <c r="A107" s="4" t="s">
         <v>176</v>
       </c>
@@ -5287,8 +5481,9 @@
       <c r="M107" s="7">
         <v>282.79000000000002</v>
       </c>
-    </row>
-    <row r="108" spans="1:13">
+      <c r="N107" s="15"/>
+    </row>
+    <row r="108" spans="1:14">
       <c r="A108" s="4" t="s">
         <v>184</v>
       </c>
@@ -5316,8 +5511,9 @@
       <c r="M108" s="7">
         <v>658.2</v>
       </c>
-    </row>
-    <row r="109" spans="1:13">
+      <c r="N108" s="15"/>
+    </row>
+    <row r="109" spans="1:14">
       <c r="A109" s="4" t="s">
         <v>190</v>
       </c>
@@ -5345,8 +5541,9 @@
       <c r="M109" s="7">
         <v>9489.34</v>
       </c>
-    </row>
-    <row r="110" spans="1:13">
+      <c r="N109" s="15"/>
+    </row>
+    <row r="110" spans="1:14">
       <c r="A110" s="4" t="s">
         <v>196</v>
       </c>
@@ -5374,8 +5571,9 @@
       <c r="M110" s="7">
         <v>957.38</v>
       </c>
-    </row>
-    <row r="111" spans="1:13">
+      <c r="N110" s="15"/>
+    </row>
+    <row r="111" spans="1:14">
       <c r="A111" s="4" t="s">
         <v>203</v>
       </c>
@@ -5403,8 +5601,9 @@
       <c r="M111" s="7">
         <v>853.28</v>
       </c>
-    </row>
-    <row r="112" spans="1:13">
+      <c r="N111" s="15"/>
+    </row>
+    <row r="112" spans="1:14">
       <c r="A112" s="4" t="s">
         <v>207</v>
       </c>
@@ -5432,6 +5631,7 @@
       <c r="M112" s="7">
         <v>1133.6099999999999</v>
       </c>
+      <c r="N112" s="15"/>
     </row>
     <row r="113" spans="1:15">
       <c r="A113" s="4" t="s">
@@ -5458,6 +5658,7 @@
       <c r="M113" s="7">
         <v>1203.28</v>
       </c>
+      <c r="N113" s="15"/>
     </row>
     <row r="114" spans="1:15">
       <c r="A114" s="4" t="s">
@@ -5484,6 +5685,7 @@
       <c r="M114" s="7">
         <v>490.16</v>
       </c>
+      <c r="N114" s="15"/>
     </row>
     <row r="115" spans="1:15">
       <c r="A115" s="4" t="s">
@@ -5510,6 +5712,7 @@
       <c r="M115" s="7">
         <v>1154.92</v>
       </c>
+      <c r="N115" s="15"/>
     </row>
     <row r="116" spans="1:15">
       <c r="A116" s="4" t="s">
@@ -5539,6 +5742,7 @@
       <c r="M116" s="7">
         <v>2367.21</v>
       </c>
+      <c r="N116" s="15"/>
     </row>
     <row r="117" spans="1:15">
       <c r="A117" s="4" t="s">
@@ -5568,6 +5772,7 @@
       <c r="M117" s="7">
         <v>3417.21</v>
       </c>
+      <c r="N117" s="15"/>
     </row>
     <row r="118" spans="1:15">
       <c r="A118" s="4" t="s">
@@ -5598,6 +5803,7 @@
       <c r="M118" s="7">
         <v>156.56</v>
       </c>
+      <c r="N118" s="15"/>
     </row>
     <row r="119" spans="1:15">
       <c r="A119" s="4" t="s">
@@ -5628,6 +5834,7 @@
       <c r="M119" s="7">
         <v>167.21</v>
       </c>
+      <c r="N119" s="15"/>
     </row>
     <row r="120" spans="1:15">
       <c r="A120" s="4" t="s">
@@ -5659,7 +5866,7 @@
       <c r="M120" s="13">
         <v>157.38</v>
       </c>
-      <c r="N120" s="6"/>
+      <c r="N120" s="15"/>
       <c r="O120" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
concluso luceplan e prova modifica colori vistosi
</commit_message>
<xml_diff>
--- a/xls/luceplan/luceplan_originario.xlsx
+++ b/xls/luceplan/luceplan_originario.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="524">
   <si>
     <t>Descrizione</t>
   </si>
@@ -1597,6 +1597,12 @@
   </si>
   <si>
     <t>D86NPI</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -2050,7 +2056,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2060,8 +2066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="I107" sqref="I107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2290,8 +2296,8 @@
       <c r="G7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="9">
-        <v>1</v>
+      <c r="J7" s="9" t="s">
+        <v>522</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>38</v>
@@ -2321,8 +2327,8 @@
       <c r="G8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="9">
-        <v>0</v>
+      <c r="J8" s="9" t="s">
+        <v>523</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>42</v>
@@ -5277,8 +5283,8 @@
       <c r="G103" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I103" s="9">
-        <v>1</v>
+      <c r="I103" s="9" t="s">
+        <v>522</v>
       </c>
       <c r="L103" s="5" t="s">
         <v>479</v>
@@ -5308,8 +5314,8 @@
       <c r="G104" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I104" s="9">
-        <v>0</v>
+      <c r="I104" s="9" t="s">
+        <v>523</v>
       </c>
       <c r="L104" s="5" t="s">
         <v>483</v>
@@ -5339,8 +5345,8 @@
       <c r="G105" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="I105" s="9">
-        <v>1</v>
+      <c r="I105" s="9" t="s">
+        <v>522</v>
       </c>
       <c r="L105" s="5" t="s">
         <v>488</v>
@@ -5370,8 +5376,8 @@
       <c r="G106" s="4" t="s">
         <v>461</v>
       </c>
-      <c r="I106" s="9">
-        <v>0</v>
+      <c r="I106" s="9" t="s">
+        <v>523</v>
       </c>
       <c r="L106" s="5" t="s">
         <v>492</v>

</xml_diff>